<commit_message>
NN needs to be corrected
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2023-05-02_L2A.xlsx
+++ b/new_modules/Summary_2023-05-02_L2A.xlsx
@@ -456,25 +456,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1199.9765625</v>
+        <v>1234.031127929688</v>
       </c>
       <c r="C2">
-        <v>0.9002</v>
+        <v>0.9258</v>
       </c>
       <c r="D2">
-        <v>0.9010000228881836</v>
+        <v>0.9351000189781189</v>
       </c>
       <c r="E2">
-        <v>1.229099988937378</v>
+        <v>1.250499963760376</v>
       </c>
       <c r="F2">
-        <v>0.5206999778747559</v>
+        <v>0.5346999764442444</v>
       </c>
       <c r="G2">
         <v>13.33</v>
       </c>
       <c r="H2">
-        <v>0.5274</v>
+        <v>0.8289</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -482,25 +482,25 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>1200.70458984375</v>
+        <v>1193.449829101562</v>
       </c>
       <c r="C3">
-        <v>0.9606</v>
+        <v>0.9548</v>
       </c>
       <c r="D3">
-        <v>0.9453</v>
+        <v>0.9539</v>
       </c>
       <c r="E3">
-        <v>1.291800022125244</v>
+        <v>1.06659996509552</v>
       </c>
       <c r="F3">
-        <v>0.6416000127792358</v>
+        <v>0.7386000156402588</v>
       </c>
       <c r="G3">
         <v>12.5</v>
       </c>
       <c r="H3">
-        <v>0.9197</v>
+        <v>0.9953</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -508,25 +508,25 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>812.0269775390625</v>
+        <v>815.7728881835938</v>
       </c>
       <c r="C4">
-        <v>0.9486</v>
+        <v>0.953</v>
       </c>
       <c r="D4">
-        <v>0.9254</v>
+        <v>0.9497</v>
       </c>
       <c r="E4">
-        <v>1.42110002040863</v>
+        <v>1.119099974632263</v>
       </c>
       <c r="F4">
-        <v>0.7505000233650208</v>
+        <v>0.756600022315979</v>
       </c>
       <c r="G4">
         <v>8.56</v>
       </c>
       <c r="H4">
-        <v>0.7433</v>
+        <v>0.9586</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -534,25 +534,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>783.861572265625</v>
+        <v>810.4166259765625</v>
       </c>
       <c r="C5">
-        <v>0.8269</v>
+        <v>0.8549</v>
       </c>
       <c r="D5">
-        <v>0.8234</v>
+        <v>0.8588</v>
       </c>
       <c r="E5">
-        <v>1.0625</v>
+        <v>1.004799962043762</v>
       </c>
       <c r="F5">
-        <v>0.4386000037193298</v>
+        <v>0.449999988079071</v>
       </c>
       <c r="G5">
         <v>9.48</v>
       </c>
       <c r="H5">
-        <v>-0.1605</v>
+        <v>0.1534</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -560,25 +560,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>1091.417114257812</v>
+        <v>1119.871948242188</v>
       </c>
       <c r="C6">
-        <v>0.8635</v>
+        <v>0.886</v>
       </c>
       <c r="D6">
-        <v>0.8669</v>
+        <v>0.8921</v>
       </c>
       <c r="E6">
-        <v>1.053799986839294</v>
+        <v>1.035400032997131</v>
       </c>
       <c r="F6">
-        <v>0.559499979019165</v>
+        <v>0.5665000081062317</v>
       </c>
       <c r="G6">
         <v>12.64</v>
       </c>
       <c r="H6">
-        <v>0.2252</v>
+        <v>0.4484</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -586,25 +586,25 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>861.890380859375</v>
+        <v>874.6599731445312</v>
       </c>
       <c r="C7">
-        <v>0.868</v>
+        <v>0.8808</v>
       </c>
       <c r="D7">
-        <v>0.8695999979972839</v>
+        <v>0.8798999786376953</v>
       </c>
       <c r="E7">
-        <v>1.012599945068359</v>
+        <v>1.01830005645752</v>
       </c>
       <c r="F7">
-        <v>0.6897000074386597</v>
+        <v>0.7138000130653381</v>
       </c>
       <c r="G7">
         <v>9.93</v>
       </c>
       <c r="H7">
-        <v>0.2493</v>
+        <v>0.3398</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -612,25 +612,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>954.7354736328125</v>
+        <v>970.0062866210938</v>
       </c>
       <c r="C8">
-        <v>0.8555</v>
+        <v>0.8692</v>
       </c>
       <c r="D8">
-        <v>0.8522999999999999</v>
+        <v>0.8683</v>
       </c>
       <c r="E8">
-        <v>1.04610002040863</v>
+        <v>1.023699998855591</v>
       </c>
       <c r="F8">
-        <v>0.7084000110626221</v>
+        <v>0.7228000164031982</v>
       </c>
       <c r="G8">
         <v>11.16</v>
       </c>
       <c r="H8">
-        <v>0.096</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -638,25 +638,25 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>6904.6123046875</v>
+        <v>7018.208984375</v>
       </c>
       <c r="C9">
-        <v>0.8898</v>
+        <v>0.9044</v>
       </c>
       <c r="D9">
-        <v>0.885</v>
+        <v>0.9121</v>
       </c>
       <c r="E9">
-        <v>1.42110002040863</v>
+        <v>1.250499963760376</v>
       </c>
       <c r="F9">
-        <v>0.4386000037193298</v>
+        <v>0.449999988079071</v>
       </c>
       <c r="G9">
         <v>77.59999999999999</v>
       </c>
       <c r="H9">
-        <v>2.6004</v>
+        <v>3.9619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NN is about to be integrated into the system
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2023-05-02_L2A.xlsx
+++ b/new_modules/Summary_2023-05-02_L2A.xlsx
@@ -456,25 +456,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1234.031127929688</v>
+        <v>1199.746215820312</v>
       </c>
       <c r="C2">
-        <v>0.9258</v>
+        <v>0.9</v>
       </c>
       <c r="D2">
-        <v>0.9351000189781189</v>
+        <v>0.9009000062942505</v>
       </c>
       <c r="E2">
-        <v>1.250499963760376</v>
+        <v>1.228800058364868</v>
       </c>
       <c r="F2">
-        <v>0.5346999764442444</v>
+        <v>0.5206000208854675</v>
       </c>
       <c r="G2">
         <v>13.33</v>
       </c>
       <c r="H2">
-        <v>0.8289</v>
+        <v>0.5258</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -482,25 +482,25 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>1193.449829101562</v>
+        <v>1200.473999023438</v>
       </c>
       <c r="C3">
-        <v>0.9548</v>
+        <v>0.9604</v>
       </c>
       <c r="D3">
-        <v>0.9539</v>
+        <v>0.9451000000000001</v>
       </c>
       <c r="E3">
-        <v>1.06659996509552</v>
+        <v>1.291599988937378</v>
       </c>
       <c r="F3">
-        <v>0.7386000156402588</v>
+        <v>0.6414999961853027</v>
       </c>
       <c r="G3">
         <v>12.5</v>
       </c>
       <c r="H3">
-        <v>0.9953</v>
+        <v>0.9181</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -508,25 +508,25 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>815.7728881835938</v>
+        <v>811.87109375</v>
       </c>
       <c r="C4">
-        <v>0.953</v>
+        <v>0.9484</v>
       </c>
       <c r="D4">
-        <v>0.9497</v>
+        <v>0.9252</v>
       </c>
       <c r="E4">
-        <v>1.119099974632263</v>
+        <v>1.420799970626831</v>
       </c>
       <c r="F4">
-        <v>0.756600022315979</v>
+        <v>0.7504000067710876</v>
       </c>
       <c r="G4">
         <v>8.56</v>
       </c>
       <c r="H4">
-        <v>0.9586</v>
+        <v>0.7417</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -534,25 +534,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>810.4166259765625</v>
+        <v>783.7109985351562</v>
       </c>
       <c r="C5">
-        <v>0.8549</v>
+        <v>0.8267</v>
       </c>
       <c r="D5">
-        <v>0.8588</v>
+        <v>0.8232</v>
       </c>
       <c r="E5">
-        <v>1.004799962043762</v>
+        <v>1.062299966812134</v>
       </c>
       <c r="F5">
-        <v>0.449999988079071</v>
+        <v>0.4384999871253967</v>
       </c>
       <c r="G5">
         <v>9.48</v>
       </c>
       <c r="H5">
-        <v>0.1534</v>
+        <v>-0.1619</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -560,25 +560,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>1119.871948242188</v>
+        <v>1091.20751953125</v>
       </c>
       <c r="C6">
-        <v>0.886</v>
+        <v>0.8633</v>
       </c>
       <c r="D6">
-        <v>0.8921</v>
+        <v>0.8668</v>
       </c>
       <c r="E6">
-        <v>1.035400032997131</v>
+        <v>1.053599953651428</v>
       </c>
       <c r="F6">
-        <v>0.5665000081062317</v>
+        <v>0.5594000220298767</v>
       </c>
       <c r="G6">
         <v>12.64</v>
       </c>
       <c r="H6">
-        <v>0.4484</v>
+        <v>0.2237</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -586,25 +586,25 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>874.6599731445312</v>
+        <v>861.7249145507812</v>
       </c>
       <c r="C7">
-        <v>0.8808</v>
+        <v>0.8678</v>
       </c>
       <c r="D7">
-        <v>0.8798999786376953</v>
+        <v>0.8694999814033508</v>
       </c>
       <c r="E7">
-        <v>1.01830005645752</v>
+        <v>1.012400031089783</v>
       </c>
       <c r="F7">
-        <v>0.7138000130653381</v>
+        <v>0.6894999742507935</v>
       </c>
       <c r="G7">
         <v>9.93</v>
       </c>
       <c r="H7">
-        <v>0.3398</v>
+        <v>0.2478</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -612,25 +612,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>970.0062866210938</v>
+        <v>954.5521240234375</v>
       </c>
       <c r="C8">
-        <v>0.8692</v>
+        <v>0.8552999999999999</v>
       </c>
       <c r="D8">
-        <v>0.8683</v>
+        <v>0.8522</v>
       </c>
       <c r="E8">
-        <v>1.023699998855591</v>
+        <v>1.045899987220764</v>
       </c>
       <c r="F8">
-        <v>0.7228000164031982</v>
+        <v>0.708299994468689</v>
       </c>
       <c r="G8">
         <v>11.16</v>
       </c>
       <c r="H8">
-        <v>0.2375</v>
+        <v>0.0946</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -638,25 +638,25 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>7018.208984375</v>
+        <v>6903.287109375</v>
       </c>
       <c r="C9">
-        <v>0.9044</v>
+        <v>0.8895999999999999</v>
       </c>
       <c r="D9">
-        <v>0.9121</v>
+        <v>0.8848</v>
       </c>
       <c r="E9">
-        <v>1.250499963760376</v>
+        <v>1.420799970626831</v>
       </c>
       <c r="F9">
-        <v>0.449999988079071</v>
+        <v>0.4384999871253967</v>
       </c>
       <c r="G9">
         <v>77.59999999999999</v>
       </c>
       <c r="H9">
-        <v>3.9619</v>
+        <v>2.589799999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>